<commit_message>
Sử dụng Service và Secret Tls trong Kubernetes
</commit_message>
<xml_diff>
--- a/trien-khai-metrics-server-tren-kubernetes/trien-khai-metrics-server-tren-kubernetes.xlsx
+++ b/trien-khai-metrics-server-tren-kubernetes/trien-khai-metrics-server-tren-kubernetes.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\kubernetes\trien-khai-metrics-server-tren-kubernetes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B97032-6826-4705-8DBD-83E1DF0B058A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43215167-3C12-4E52-BB64-EB564B20200D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="metrics server" sheetId="1" r:id="rId1"/>
-    <sheet name="Check Dashboard" sheetId="2" r:id="rId2"/>
+    <sheet name="Installation" sheetId="3" r:id="rId1"/>
+    <sheet name="metrics server" sheetId="1" r:id="rId2"/>
+    <sheet name="Check Dashboard" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Kiểm tra các pod</t>
   </si>
@@ -126,6 +127,12 @@
       </rPr>
       <t xml:space="preserve"> Cần có Metric Server để HPA hoạt động chính xác</t>
     </r>
+  </si>
+  <si>
+    <t>kubectl apply -f https://github.com/kubernetes-sigs/metrics-server/releases/latest/download/components.yaml</t>
+  </si>
+  <si>
+    <t>Installation</t>
   </si>
 </sst>
 </file>
@@ -811,11 +818,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{101D7FC6-F7F9-4063-A81D-2ED9B1CB7C39}">
+  <dimension ref="A2:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:B117"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="B104" sqref="B104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -912,11 +944,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE72C55F-80E1-403D-A90F-EB9A4C4EB810}">
   <dimension ref="A2:A30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>

</xml_diff>